<commit_message>
update stim bank, gitignore, and .psyexp file
</commit_message>
<xml_diff>
--- a/stimulus_bank.xlsx
+++ b/stimulus_bank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkoen/Documents/GitHub/emo-gonogo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3841361A-BDB3-A74B-9D2F-94E77EFE61FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A140F2-BC17-C449-9A02-685541B7B25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iaps_stimuli" sheetId="9" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="829">
   <si>
     <t>photo</t>
   </si>
@@ -2594,7 +2594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2616,6 +2616,22 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -16459,14 +16475,1134 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6F5D4-93CD-0648-B78B-0EFD3B0736B7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>A2&amp;".jpg"</f>
+        <v>Animals_001_h.jpg</v>
+      </c>
+      <c r="C2" s="13">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3.25</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.18</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3.55</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>A3&amp;".jpg"</f>
+        <v>Animals_009_v.jpg</v>
+      </c>
+      <c r="C3" s="18">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>5.2</v>
+      </c>
+      <c r="E3" s="14">
+        <v>1.41</v>
+      </c>
+      <c r="F3" s="14">
+        <v>3.5</v>
+      </c>
+      <c r="G3" s="14">
+        <v>2.09</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>A4&amp;".jpg"</f>
+        <v>Animals_039_h.jpg</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.92</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F4" s="4">
+        <v>6.33</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1.85</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>A5&amp;".jpg"</f>
+        <v>Animals_060_h.jpg</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.08</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.69</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2.06</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>A6&amp;".jpg"</f>
+        <v>Animals_085_h.jpg</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>5.08</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1.64</v>
+      </c>
+      <c r="F6" s="14">
+        <v>4.49</v>
+      </c>
+      <c r="G6" s="14">
+        <v>2.19</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>A7&amp;".jpg"</f>
+        <v>Animals_089_v.jpg</v>
+      </c>
+      <c r="C7" s="18">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14">
+        <v>5.72</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1.17</v>
+      </c>
+      <c r="F7" s="14">
+        <v>2.74</v>
+      </c>
+      <c r="G7" s="14">
+        <v>1.86</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>A8&amp;".jpg"</f>
+        <v>Animals_122_h.jpg</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>6.18</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1.06</v>
+      </c>
+      <c r="F8" s="14">
+        <v>2.95</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1.51</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>A9&amp;".jpg"</f>
+        <v>Animals_135_v.jpg</v>
+      </c>
+      <c r="C9" s="18">
+        <v>2</v>
+      </c>
+      <c r="D9" s="14">
+        <v>5.12</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1.05</v>
+      </c>
+      <c r="F9" s="14">
+        <v>2.77</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1.94</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>A10&amp;".jpg"</f>
+        <v>Animals_171_h.jpg</v>
+      </c>
+      <c r="C10" s="18">
+        <v>3</v>
+      </c>
+      <c r="D10" s="14">
+        <v>5.41</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1.61</v>
+      </c>
+      <c r="F10" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="G10" s="14">
+        <v>2.11</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>A11&amp;".jpg"</f>
+        <v>Animals_182_h.jpg</v>
+      </c>
+      <c r="C11" s="18">
+        <v>2</v>
+      </c>
+      <c r="D11" s="14">
+        <v>5.68</v>
+      </c>
+      <c r="E11" s="14">
+        <v>1.18</v>
+      </c>
+      <c r="F11" s="14">
+        <v>2.57</v>
+      </c>
+      <c r="G11" s="14">
+        <v>1.48</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>A12&amp;".jpg"</f>
+        <v>Animals_217_h.jpg</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14">
+        <v>5.79</v>
+      </c>
+      <c r="E12" s="14">
+        <v>1.61</v>
+      </c>
+      <c r="F12" s="14">
+        <v>2.62</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1.6</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>A13&amp;".jpg"</f>
+        <v>Faces_007_h.jpg</v>
+      </c>
+      <c r="C13" s="13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2.35</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.02</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2.17</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>A14&amp;".jpg"</f>
+        <v>Faces_066_h.jpg</v>
+      </c>
+      <c r="C14" s="18">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14">
+        <v>6.87</v>
+      </c>
+      <c r="E14" s="14">
+        <v>1.22</v>
+      </c>
+      <c r="F14" s="14">
+        <v>3.23</v>
+      </c>
+      <c r="G14" s="14">
+        <v>1.97</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <f>A15&amp;".jpg"</f>
+        <v>Faces_088_v.jpg</v>
+      </c>
+      <c r="C15" s="18">
+        <v>2</v>
+      </c>
+      <c r="D15" s="14">
+        <v>6.14</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="F15" s="14">
+        <v>2.93</v>
+      </c>
+      <c r="G15" s="14">
+        <v>1.84</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f>A16&amp;".jpg"</f>
+        <v>Faces_138_h.jpg</v>
+      </c>
+      <c r="C16" s="18">
+        <v>3</v>
+      </c>
+      <c r="D16" s="14">
+        <v>5.55</v>
+      </c>
+      <c r="E16" s="14">
+        <v>1.01</v>
+      </c>
+      <c r="F16" s="14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G16" s="14">
+        <v>1.71</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>A17&amp;".jpg"</f>
+        <v>Faces_140_h.jpg</v>
+      </c>
+      <c r="C17" s="18">
+        <v>3</v>
+      </c>
+      <c r="D17" s="14">
+        <v>6.12</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1.29</v>
+      </c>
+      <c r="F17" s="14">
+        <v>2.68</v>
+      </c>
+      <c r="G17" s="14">
+        <v>1.86</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f>A18&amp;".jpg"</f>
+        <v>Faces_158_h.jpg</v>
+      </c>
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3.28</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.36</v>
+      </c>
+      <c r="F18" s="4">
+        <v>3.64</v>
+      </c>
+      <c r="G18" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="str">
+        <f>A19&amp;".jpg"</f>
+        <v>Faces_273_h.jpg</v>
+      </c>
+      <c r="C19" s="13">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3.72</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1.82</v>
+      </c>
+      <c r="F19" s="4">
+        <v>3.95</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2.06</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f>A20&amp;".jpg"</f>
+        <v>Faces_288_h.jpg</v>
+      </c>
+      <c r="C20" s="13">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3.33</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1.51</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3.82</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2.04</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f>A21&amp;".jpg"</f>
+        <v>Faces_340_h.jpg</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1</v>
+      </c>
+      <c r="D21" s="14">
+        <v>6.92</v>
+      </c>
+      <c r="E21" s="14">
+        <v>1.42</v>
+      </c>
+      <c r="F21" s="14">
+        <v>3.64</v>
+      </c>
+      <c r="G21" s="14">
+        <v>2.68</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f>A22&amp;".jpg"</f>
+        <v>Faces_350_h.jpg</v>
+      </c>
+      <c r="C22" s="19">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>6.49</v>
+      </c>
+      <c r="E22">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F22">
+        <v>2.89</v>
+      </c>
+      <c r="G22">
+        <v>1.73</v>
+      </c>
+      <c r="H22" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2" t="str">
+        <f>A23&amp;".jpg"</f>
+        <v>Faces_351_h.jpg</v>
+      </c>
+      <c r="C23" s="19">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>6.56</v>
+      </c>
+      <c r="E23">
+        <v>1.43</v>
+      </c>
+      <c r="F23">
+        <v>2.83</v>
+      </c>
+      <c r="G23">
+        <v>1.87</v>
+      </c>
+      <c r="H23" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f>A24&amp;".jpg"</f>
+        <v>Faces_357_v.jpg</v>
+      </c>
+      <c r="C24" s="19">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>6.1</v>
+      </c>
+      <c r="E24">
+        <v>1.47</v>
+      </c>
+      <c r="F24">
+        <v>2.87</v>
+      </c>
+      <c r="G24">
+        <v>1.59</v>
+      </c>
+      <c r="H24" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f>A25&amp;".jpg"</f>
+        <v>Faces_363_v.jpg</v>
+      </c>
+      <c r="C25" s="20">
+        <v>3</v>
+      </c>
+      <c r="D25" s="16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E25" s="16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F25" s="17">
+        <v>4.22</v>
+      </c>
+      <c r="G25" s="16">
+        <v>2.12</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f>A26&amp;".jpg"</f>
+        <v>Landscapes_005_h.jpg</v>
+      </c>
+      <c r="C26" s="20">
+        <v>2</v>
+      </c>
+      <c r="D26" s="16">
+        <v>3.73</v>
+      </c>
+      <c r="E26" s="16">
+        <v>1.35</v>
+      </c>
+      <c r="F26" s="16">
+        <v>3.68</v>
+      </c>
+      <c r="G26" s="16">
+        <v>2.16</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="str">
+        <f>A27&amp;".jpg"</f>
+        <v>Landscapes_119_h.jpg</v>
+      </c>
+      <c r="C27" s="19">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>6.03</v>
+      </c>
+      <c r="E27">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="F27">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="G27">
+        <v>1.28</v>
+      </c>
+      <c r="H27" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2" t="str">
+        <f>A28&amp;".jpg"</f>
+        <v>Objects_007_h.jpg</v>
+      </c>
+      <c r="C28" s="20">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16">
+        <v>3.62</v>
+      </c>
+      <c r="E28" s="16">
+        <v>1.55</v>
+      </c>
+      <c r="F28" s="16">
+        <v>3.69</v>
+      </c>
+      <c r="G28" s="16">
+        <v>2.25</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f>A29&amp;".jpg"</f>
+        <v>Objects_154_h.jpg</v>
+      </c>
+      <c r="C29" s="20">
+        <v>1</v>
+      </c>
+      <c r="D29" s="16">
+        <v>3.59</v>
+      </c>
+      <c r="E29" s="16">
+        <v>1.52</v>
+      </c>
+      <c r="F29" s="16">
+        <v>3.64</v>
+      </c>
+      <c r="G29" s="16">
+        <v>1.87</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2" t="str">
+        <f>A30&amp;".jpg"</f>
+        <v>Objects_195_v.jpg</v>
+      </c>
+      <c r="C30" s="19">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>5.31</v>
+      </c>
+      <c r="E30">
+        <v>1.38</v>
+      </c>
+      <c r="F30">
+        <v>2.34</v>
+      </c>
+      <c r="G30">
+        <v>1.48</v>
+      </c>
+      <c r="H30" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2" t="str">
+        <f>A31&amp;".jpg"</f>
+        <v>Objects_244_h.jpg</v>
+      </c>
+      <c r="C31" s="19">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>5.35</v>
+      </c>
+      <c r="E31">
+        <v>1.21</v>
+      </c>
+      <c r="F31">
+        <v>2.75</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2" t="str">
+        <f>A32&amp;".jpg"</f>
+        <v>Objects_249_v.jpg</v>
+      </c>
+      <c r="C32" s="19">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>5.18</v>
+      </c>
+      <c r="E32">
+        <v>0.79</v>
+      </c>
+      <c r="F32">
+        <v>2.02</v>
+      </c>
+      <c r="G32">
+        <v>1.21</v>
+      </c>
+      <c r="H32" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <f>A33&amp;".jpg"</f>
+        <v>Objects_285_h.jpg</v>
+      </c>
+      <c r="C33" s="20">
+        <v>3</v>
+      </c>
+      <c r="D33" s="16">
+        <v>3.17</v>
+      </c>
+      <c r="E33" s="16">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F33" s="16">
+        <v>3.56</v>
+      </c>
+      <c r="G33" s="16">
+        <v>2.12</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2" t="str">
+        <f>A34&amp;".jpg"</f>
+        <v>People_016_h.jpg</v>
+      </c>
+      <c r="C34" s="20">
+        <v>3</v>
+      </c>
+      <c r="D34" s="16">
+        <v>2.85</v>
+      </c>
+      <c r="E34" s="16">
+        <v>1.35</v>
+      </c>
+      <c r="F34" s="16">
+        <v>3.8</v>
+      </c>
+      <c r="G34" s="16">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="2" t="str">
+        <f>A35&amp;".jpg"</f>
+        <v>People_198_h.jpg</v>
+      </c>
+      <c r="C35" s="20">
+        <v>3</v>
+      </c>
+      <c r="D35" s="16">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E35" s="16">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="F35" s="16">
+        <v>5.32</v>
+      </c>
+      <c r="G35" s="16">
+        <v>2.44</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2" t="str">
+        <f>A36&amp;".jpg"</f>
+        <v>People_201_v.jpg</v>
+      </c>
+      <c r="C36" s="20">
+        <v>1</v>
+      </c>
+      <c r="D36" s="16">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="E36" s="16">
+        <v>1.31</v>
+      </c>
+      <c r="F36" s="16">
+        <v>5.05</v>
+      </c>
+      <c r="G36" s="16">
+        <v>2.25</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="2" t="str">
+        <f>A37&amp;".jpg"</f>
+        <v>People_202_h.jpg</v>
+      </c>
+      <c r="C37" s="20">
+        <v>1</v>
+      </c>
+      <c r="D37" s="16">
+        <v>2.79</v>
+      </c>
+      <c r="E37" s="16">
+        <v>1.63</v>
+      </c>
+      <c r="F37" s="16">
+        <v>5.87</v>
+      </c>
+      <c r="G37" s="16">
+        <v>2.27</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2" t="str">
+        <f>A38&amp;".jpg"</f>
+        <v>People_217_h.jpg</v>
+      </c>
+      <c r="C38" s="20">
+        <v>1</v>
+      </c>
+      <c r="D38" s="16">
+        <v>3.08</v>
+      </c>
+      <c r="E38" s="16">
+        <v>1.55</v>
+      </c>
+      <c r="F38" s="16">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="G38" s="16">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="2" t="str">
+        <f>A39&amp;".jpg"</f>
+        <v>People_223_h.jpg</v>
+      </c>
+      <c r="C39" s="20">
+        <v>3</v>
+      </c>
+      <c r="D39" s="16">
+        <v>3.51</v>
+      </c>
+      <c r="E39" s="16">
+        <v>1.52</v>
+      </c>
+      <c r="F39" s="16">
+        <v>4.22</v>
+      </c>
+      <c r="G39" s="16">
+        <v>2.39</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="2" t="str">
+        <f>A40&amp;".jpg"</f>
+        <v>People_225_h.jpg</v>
+      </c>
+      <c r="C40" s="20">
+        <v>3</v>
+      </c>
+      <c r="D40" s="16">
+        <v>3.02</v>
+      </c>
+      <c r="E40" s="16">
+        <v>1.17</v>
+      </c>
+      <c r="F40" s="16">
+        <v>3.76</v>
+      </c>
+      <c r="G40" s="16">
+        <v>2.19</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="2" t="str">
+        <f>A41&amp;".jpg"</f>
+        <v>People_239_h.jpg</v>
+      </c>
+      <c r="C41" s="20">
+        <v>1</v>
+      </c>
+      <c r="D41" s="16">
+        <v>2.21</v>
+      </c>
+      <c r="E41" s="16">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F41" s="16">
+        <v>5.74</v>
+      </c>
+      <c r="G41" s="16">
+        <v>2.17</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H41">
+    <sortCondition ref="A1:A41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16475,8 +17611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85792C83-307D-B648-BA95-DCA17291481F}">
   <dimension ref="A1:S104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:M5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -19098,7 +20234,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:M5"/>
+      <selection activeCell="A2" sqref="A2:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>